<commit_message>
changes to epiet cs
Update epiet
</commit_message>
<xml_diff>
--- a/cs/ENG/stengen_mva/data/data_dictionary_stengen_mva.xlsx
+++ b/cs/ENG/stengen_mva/data/data_dictionary_stengen_mva.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateourdiales_albert\Documents\EPIET\stengen_mva\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateourdiales_albert\Documents\GitHub\case_studies\cs\ENG\stengen_mva\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBD4563-5CF7-4C44-8014-803B766F417D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776500EF-8664-42D7-B71A-4FFE5CD1FA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{74A010DD-C908-4C20-891B-850BE9625381}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74A010DD-C908-4C20-891B-850BE9625381}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Column</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>dmousse</t>
-  </si>
-  <si>
-    <t>mousse</t>
   </si>
   <si>
     <t>mportion</t>
@@ -194,18 +191,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -220,9 +211,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -558,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B635FE-FF0D-4C3E-8882-CA86E859B986}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -572,13 +562,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -601,7 +591,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -634,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -653,10 +643,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -664,138 +654,131 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>